<commit_message>
WIP: Testing new read_gcwerks_flask function
</commit_message>
<xml_diff>
--- a/data/cbwflask/data_release_schedule.xlsx
+++ b/data/cbwflask/data_release_schedule.xlsx
@@ -5,17 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chxmr/code/template-archive/data/project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chxmr/code/cbw-flask-archive/data/cbwflask/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC900837-8265-044F-8EE7-0725D85C3F57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B62DCC2-8DD8-6F4B-AC6E-95FF64B17A01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11160" yWindow="500" windowWidth="27240" windowHeight="16440" xr2:uid="{D0121EA7-C121-5646-A290-A6B31742EFF2}"/>
   </bookViews>
   <sheets>
-    <sheet name="GCMD" sheetId="1" r:id="rId1"/>
-    <sheet name="Picarro" sheetId="8" r:id="rId2"/>
-    <sheet name="LGR" sheetId="11" r:id="rId3"/>
+    <sheet name="GCMS-Medusa-flask" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t># DO NOT CHANGE THE FORMAT OF THIS SPREADSHEET</t>
   </si>
@@ -46,15 +44,9 @@
     <t># Date format YYYY-MM-DD HH:MM</t>
   </si>
   <si>
-    <t># AGAGE GCMD data release schedule</t>
-  </si>
-  <si>
     <t>General release date</t>
   </si>
   <si>
-    <t>2023-01-01 00:00</t>
-  </si>
-  <si>
     <t>Species</t>
   </si>
   <si>
@@ -67,17 +59,143 @@
     <t># All data will be processed until the "general release date" unless specified in the table</t>
   </si>
   <si>
-    <t>BSD</t>
-  </si>
-  <si>
-    <t>TAC</t>
+    <t>CBW</t>
+  </si>
+  <si>
+    <t>2024-01-01 00:00</t>
+  </si>
+  <si>
+    <t># AGAGE GCM-Medusa-flask data release schedule</t>
+  </si>
+  <si>
+    <t>hfc-23</t>
+  </si>
+  <si>
+    <t>hfc-32</t>
+  </si>
+  <si>
+    <t>hfc-125</t>
+  </si>
+  <si>
+    <t>hfc-134a</t>
+  </si>
+  <si>
+    <t>hfc-143a</t>
+  </si>
+  <si>
+    <t>hfc-152a</t>
+  </si>
+  <si>
+    <t>hfc-227ea</t>
+  </si>
+  <si>
+    <t>hfc-236fa</t>
+  </si>
+  <si>
+    <t>hfc-245fa</t>
+  </si>
+  <si>
+    <t>hfc-365mfc</t>
+  </si>
+  <si>
+    <t>hfc-4310mee</t>
+  </si>
+  <si>
+    <t>hcfc-22</t>
+  </si>
+  <si>
+    <t>hcfc-124</t>
+  </si>
+  <si>
+    <t>hcfc-132b</t>
+  </si>
+  <si>
+    <t>hcfc-133a</t>
+  </si>
+  <si>
+    <t>hcfc-141b</t>
+  </si>
+  <si>
+    <t>hcfc-142b</t>
+  </si>
+  <si>
+    <t>cfc-11</t>
+  </si>
+  <si>
+    <t>cfc-12</t>
+  </si>
+  <si>
+    <t>cfc-13</t>
+  </si>
+  <si>
+    <t>cfc-113</t>
+  </si>
+  <si>
+    <t>cfc-114</t>
+  </si>
+  <si>
+    <t>cfc-115</t>
+  </si>
+  <si>
+    <t>h-1211</t>
+  </si>
+  <si>
+    <t>h-1301</t>
+  </si>
+  <si>
+    <t>h-2402</t>
+  </si>
+  <si>
+    <t>ch3cl</t>
+  </si>
+  <si>
+    <t>ch3br</t>
+  </si>
+  <si>
+    <t>ch2cl2</t>
+  </si>
+  <si>
+    <t>chcl3</t>
+  </si>
+  <si>
+    <t>ch3ccl3</t>
+  </si>
+  <si>
+    <t>ccl4</t>
+  </si>
+  <si>
+    <t>tce</t>
+  </si>
+  <si>
+    <t>pce</t>
+  </si>
+  <si>
+    <t>sf6</t>
+  </si>
+  <si>
+    <t>so2f2</t>
+  </si>
+  <si>
+    <t>nf3</t>
+  </si>
+  <si>
+    <t>cf4</t>
+  </si>
+  <si>
+    <t>c2f6</t>
+  </si>
+  <si>
+    <t>c3f8</t>
+  </si>
+  <si>
+    <t>c4f8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -93,6 +211,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -102,7 +226,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -130,17 +254,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -151,7 +264,7 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -466,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F54C872C-8629-284F-A579-6B1D027BD782}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="114" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -480,7 +593,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -490,7 +603,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -500,158 +613,233 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B5DB9A0-5433-FF47-BABC-7C9213421903}">
-  <dimension ref="A1:B8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="20" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.83203125" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E362F148-5D79-214D-93BA-FD6AF7AFDC2B}">
-  <dimension ref="A1:B8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="20" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.83203125" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="5" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" s="5" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bug fixes, and updates to Readme files
</commit_message>
<xml_diff>
--- a/data/cbwflask/data_release_schedule.xlsx
+++ b/data/cbwflask/data_release_schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chxmr/code/cbw-flask-archive/data/cbwflask/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B62DCC2-8DD8-6F4B-AC6E-95FF64B17A01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37327745-60C0-584F-9052-2E8FD8E14D2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11160" yWindow="500" windowWidth="27240" windowHeight="16440" xr2:uid="{D0121EA7-C121-5646-A290-A6B31742EFF2}"/>
+    <workbookView xWindow="3000" yWindow="760" windowWidth="27240" windowHeight="16440" xr2:uid="{D0121EA7-C121-5646-A290-A6B31742EFF2}"/>
   </bookViews>
   <sheets>
     <sheet name="GCMS-Medusa-flask" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t># DO NOT CHANGE THE FORMAT OF THIS SPREADSHEET</t>
   </si>
@@ -189,6 +189,9 @@
   </si>
   <si>
     <t>c4f8</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -581,8 +584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F54C872C-8629-284F-A579-6B1D027BD782}">
   <dimension ref="A1:B49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="114" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="114" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -757,82 +760,85 @@
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B41" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
         <v>49</v>
       </c>

</xml_diff>